<commit_message>
all first three test cases run succesfully
</commit_message>
<xml_diff>
--- a/data/xinyangapitesting own.xlsx
+++ b/data/xinyangapitesting own.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyangzhang/Documents/Pycharm/API-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9456A9DE-CE72-FD46-8DFC-E4237F4D27DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882E9C43-D479-B54E-982B-AD06684B4543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="8220" windowWidth="42040" windowHeight="18800" activeTab="1" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
+    <workbookView xWindow="-36500" yWindow="4760" windowWidth="31640" windowHeight="18800" activeTab="1" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
   </bookViews>
   <sheets>
     <sheet name="test_register" sheetId="3" r:id="rId1"/>
@@ -268,35 +268,6 @@
     <t>{"principal": "", "credentials": "lemon123456", "appType": 3, "loginType": 0}</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>{"text":"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>账号或密码不正确</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>"}</t>
-    </r>
-  </si>
-  <si>
     <t>{"principal": "lem", "credentials": "lemon123456", "appType": 3, "loginType": 0}</t>
   </si>
   <si>
@@ -492,13 +463,16 @@
   </si>
   <si>
     <t>{"addrId": 0, "basketIds":[#basketId#], "couponIds": [], "isScorePay": 0, "userChangeCoupon": 0,       "userUseScore": 0}</t>
+  </si>
+  <si>
+    <t>{"text":"Incorrect account or password"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -552,12 +526,6 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -615,7 +583,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -955,11 +923,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70910427-306D-C74C-9DEC-96EC5E562EFF}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.83203125" customWidth="1"/>
     <col min="2" max="2" width="45.33203125" customWidth="1"/>
@@ -972,7 +940,7 @@
     <col min="9" max="9" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -998,76 +966,76 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="85">
+    </row>
+    <row r="3" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="51">
+    </row>
+    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
         <v>69</v>
       </c>
-      <c r="E4" t="s">
-        <v>70</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1085,21 +1053,21 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="46" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="35.83203125" customWidth="1"/>
     <col min="5" max="5" width="35.6640625" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="6" max="6" width="43.5" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
     <col min="8" max="8" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1128,15 +1096,15 @@
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="51">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -1155,12 +1123,12 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="51">
+    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>9</v>
@@ -1175,16 +1143,16 @@
         <v>41</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="51">
+    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
@@ -1196,18 +1164,18 @@
         <v>37</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="62" customHeight="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -1219,18 +1187,18 @@
         <v>37</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="51">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>9</v>
@@ -1242,18 +1210,18 @@
         <v>37</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="51">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>9</v>
@@ -1265,18 +1233,18 @@
         <v>37</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="51">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>9</v>
@@ -1288,18 +1256,18 @@
         <v>37</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="51">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
@@ -1311,10 +1279,10 @@
         <v>37</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1336,11 +1304,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562F5F3D-E2EA-9240-9A70-317BC054BC3A}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="29.5" customWidth="1"/>
@@ -1353,7 +1321,7 @@
     <col min="9" max="9" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1382,10 +1350,10 @@
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="34">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1408,10 +1376,10 @@
         <v>12</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1422,7 +1390,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
@@ -1431,7 +1399,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17">
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1445,13 +1413,13 @@
         <v>17</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="66" customHeight="1">
+    <row r="5" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1468,10 +1436,10 @@
         <v>30</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="61" customHeight="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1494,7 +1462,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="32">
+    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1511,10 +1479,10 @@
         <v>30</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="136">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="136" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
added db assertion method
</commit_message>
<xml_diff>
--- a/data/xinyangapitesting own.xlsx
+++ b/data/xinyangapitesting own.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyangzhang/Documents/Pycharm/API-Automation/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mycodefiles\pythoncodefiles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882E9C43-D479-B54E-982B-AD06684B4543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192F8428-1C6D-4BE9-B0A6-B903543DA7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36500" yWindow="4760" windowWidth="31640" windowHeight="18800" activeTab="1" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
+    <workbookView xWindow="320" yWindow="12640" windowWidth="17930" windowHeight="10710" activeTab="2" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
   </bookViews>
   <sheets>
     <sheet name="test_register" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="96">
   <si>
     <t>url</t>
   </si>
@@ -466,13 +466,187 @@
   </si>
   <si>
     <t>{"text":"Incorrect account or password"}</t>
+  </si>
+  <si>
+    <t>http://shop.lemonban.com:8107/notice/pay/3</t>
+  </si>
+  <si>
+    <t>mock payment callback</t>
+  </si>
+  <si>
+    <t>make payment</t>
+  </si>
+  <si>
+    <t>http://shop.lemonban.com:8107/p/order/pay</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>{"Content-Type":"application/json","Authorization": "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#token_type##access_token#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>{"payType":3,"orderNumbers":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>orderNumbers#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>{"payNo":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>orderNumbers#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>","bizPayNo":"XXX","isPaySuccess":true}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">check the order status </t>
+  </si>
+  <si>
+    <t>http://shop.lemonban.com:8107/p/order/isPay/#orderNumbers#</t>
+  </si>
+  <si>
+    <t>{"text":"true"}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>{"select status from tz_order where order_number = '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>#orderNumbers#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>'":2,"select is_payed from tz_order where order_number = '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>#orderNumbers#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>'":1}</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -533,6 +707,32 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -561,7 +761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -584,6 +784,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -927,20 +1136,20 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="45.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="47.5" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" customWidth="1"/>
-    <col min="6" max="6" width="57.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="24.1640625" customWidth="1"/>
-    <col min="9" max="9" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.84375" customWidth="1"/>
+    <col min="2" max="2" width="45.3046875" customWidth="1"/>
+    <col min="3" max="3" width="21.4609375" customWidth="1"/>
+    <col min="4" max="4" width="47.4609375" customWidth="1"/>
+    <col min="5" max="5" width="42.69140625" customWidth="1"/>
+    <col min="6" max="6" width="57.69140625" customWidth="1"/>
+    <col min="7" max="7" width="25.4609375" customWidth="1"/>
+    <col min="8" max="8" width="24.15234375" customWidth="1"/>
+    <col min="9" max="9" width="34.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -972,7 +1181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -992,7 +1201,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="77.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1018,7 +1227,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="46.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1052,22 +1261,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F1B2B2-99C6-F74C-BE60-04C41AAB74CA}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <cols>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="35.83203125" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" customWidth="1"/>
-    <col min="6" max="6" width="43.5" customWidth="1"/>
-    <col min="7" max="7" width="31.5" customWidth="1"/>
-    <col min="8" max="8" width="34.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.4609375" customWidth="1"/>
+    <col min="4" max="4" width="35.84375" customWidth="1"/>
+    <col min="5" max="5" width="35.69140625" customWidth="1"/>
+    <col min="6" max="6" width="43.4609375" customWidth="1"/>
+    <col min="7" max="7" width="31.4609375" customWidth="1"/>
+    <col min="8" max="8" width="34.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1099,7 +1308,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="31">
       <c r="A2" s="7" t="s">
         <v>48</v>
       </c>
@@ -1123,7 +1332,7 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="31">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -1147,7 +1356,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="31">
       <c r="A4" s="7" t="s">
         <v>50</v>
       </c>
@@ -1170,7 +1379,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="62" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>51</v>
       </c>
@@ -1193,7 +1402,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="31">
       <c r="A6" s="7" t="s">
         <v>52</v>
       </c>
@@ -1216,7 +1425,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="31">
       <c r="A7" s="7" t="s">
         <v>53</v>
       </c>
@@ -1239,7 +1448,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="31">
       <c r="A8" s="7" t="s">
         <v>54</v>
       </c>
@@ -1262,7 +1471,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="31">
       <c r="A9" s="7" t="s">
         <v>55</v>
       </c>
@@ -1302,26 +1511,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562F5F3D-E2EA-9240-9A70-317BC054BC3A}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="47" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" customWidth="1"/>
-    <col min="5" max="5" width="60.83203125" customWidth="1"/>
-    <col min="6" max="6" width="49.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.4609375" customWidth="1"/>
+    <col min="3" max="3" width="9.15234375" customWidth="1"/>
+    <col min="4" max="4" width="46.3046875" customWidth="1"/>
+    <col min="5" max="5" width="60.84375" customWidth="1"/>
+    <col min="6" max="6" width="49.15234375" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
-    <col min="8" max="8" width="34.33203125" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="34.3046875" customWidth="1"/>
+    <col min="9" max="9" width="21.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1353,7 +1562,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="31">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1379,7 +1588,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1399,7 +1608,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1419,7 +1628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="66" customHeight="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1439,7 +1648,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="61" customHeight="1">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1462,9 +1671,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="29">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -1482,9 +1691,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="136" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="124">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
@@ -1509,6 +1718,70 @@
       </c>
       <c r="I8" s="3" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="29">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="29">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="120">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1518,6 +1791,9 @@
     <hyperlink ref="D6" r:id="rId3" xr:uid="{C52EC358-BD85-4A44-8128-30A17D00202F}"/>
     <hyperlink ref="D8" r:id="rId4" xr:uid="{E707AACC-01C5-CA4F-A462-67DAB27B3CA3}"/>
     <hyperlink ref="D3" r:id="rId5" xr:uid="{A53AEE31-FA46-4A4F-ACE4-E20E86943EFA}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{93966403-D63E-4883-AFAE-F6E4D454E123}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{7A949514-4B2C-4394-A4A1-DBA4049BFADA}"/>
+    <hyperlink ref="D11" r:id="rId8" location="orderNumbers#" xr:uid="{06BBD282-F827-4994-BD6F-07980F9ADE15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updated some data add replace method for URL more notes on allure added
</commit_message>
<xml_diff>
--- a/data/xinyangapitesting own.xlsx
+++ b/data/xinyangapitesting own.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mycodefiles\pythoncodefiles\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13091\PycharmProjects\API-Automation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192F8428-1C6D-4BE9-B0A6-B903543DA7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979AF455-007A-429D-B315-70D6F7C497CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="12640" windowWidth="17930" windowHeight="10710" activeTab="2" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
+    <workbookView xWindow="-110" yWindow="11890" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
   </bookViews>
   <sheets>
     <sheet name="test_register" sheetId="3" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>http://shop.lemonban.com:8107/login</t>
   </si>
   <si>
-    <t>{"principal":"lemon_py","credentials":"12345678","appType":3,"loginType":0}</t>
-  </si>
-  <si>
     <t>{"nickName": "lemon_py","enabled": true}</t>
   </si>
   <si>
@@ -259,12 +256,6 @@
     <t>request_parameter</t>
   </si>
   <si>
-    <t>{"principal": "lemon_py", "credentials": "12345678", "appType": 3, "loginType": 0}</t>
-  </si>
-  <si>
-    <t>{"$..nickName":"lemon_py","$..enabled":true}</t>
-  </si>
-  <si>
     <t>{"principal": "", "credentials": "lemon123456", "appType": 3, "loginType": 0}</t>
   </si>
   <si>
@@ -463,9 +454,6 @@
   </si>
   <si>
     <t>{"addrId": 0, "basketIds":[#basketId#], "couponIds": [], "isScorePay": 0, "userChangeCoupon": 0,       "userUseScore": 0}</t>
-  </si>
-  <si>
-    <t>{"text":"Incorrect account or password"}</t>
   </si>
   <si>
     <t>http://shop.lemonban.com:8107/notice/pay/3</t>
@@ -640,6 +628,18 @@
       </rPr>
       <t>'":1}</t>
     </r>
+  </si>
+  <si>
+    <t>{"principal":"lemonxinyang","credentials":"Ginny_1212","appType":3,"loginType":0}</t>
+  </si>
+  <si>
+    <t>{"principal": "lemonxinyang", "credentials": "Ginny_1212", "appType": 3, "loginType": 0}</t>
+  </si>
+  <si>
+    <t>{"$..nickName":"lemonxinyang","$..enabled":true}</t>
+  </si>
+  <si>
+    <t>{"text":"账号或密码不正确"}</t>
   </si>
 </sst>
 </file>
@@ -1132,21 +1132,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70910427-306D-C74C-9DEC-96EC5E562EFF}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="22.84375" customWidth="1"/>
-    <col min="2" max="2" width="45.3046875" customWidth="1"/>
-    <col min="3" max="3" width="21.4609375" customWidth="1"/>
-    <col min="4" max="4" width="47.4609375" customWidth="1"/>
-    <col min="5" max="5" width="42.69140625" customWidth="1"/>
-    <col min="6" max="6" width="57.69140625" customWidth="1"/>
-    <col min="7" max="7" width="25.4609375" customWidth="1"/>
-    <col min="8" max="8" width="24.15234375" customWidth="1"/>
-    <col min="9" max="9" width="34.84375" customWidth="1"/>
+    <col min="1" max="1" width="14.4140625" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="47.5" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="6" max="6" width="57.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" customWidth="1"/>
+    <col min="9" max="9" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1">
@@ -1166,7 +1166,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1175,7 +1175,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
@@ -1186,65 +1186,65 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="F2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="77.5">
+    </row>
+    <row r="3" spans="1:10" ht="80">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" t="s">
         <v>70</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="46.5">
+    </row>
+    <row r="4" spans="1:10" ht="48">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1261,19 +1261,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F1B2B2-99C6-F74C-BE60-04C41AAB74CA}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="23.4609375" customWidth="1"/>
-    <col min="4" max="4" width="35.84375" customWidth="1"/>
-    <col min="5" max="5" width="35.69140625" customWidth="1"/>
-    <col min="6" max="6" width="43.4609375" customWidth="1"/>
-    <col min="7" max="7" width="31.4609375" customWidth="1"/>
-    <col min="8" max="8" width="34.15234375" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="43.5" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
+    <col min="8" max="8" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1">
@@ -1293,7 +1293,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1305,15 +1305,15 @@
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="31">
       <c r="A2" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -1322,22 +1322,22 @@
         <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:10" ht="31">
       <c r="A3" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>9</v>
@@ -1346,22 +1346,22 @@
         <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="31">
       <c r="A4" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
@@ -1370,21 +1370,21 @@
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="62" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -1393,21 +1393,21 @@
         <v>10</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="31">
       <c r="A6" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>9</v>
@@ -1416,21 +1416,21 @@
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="31">
       <c r="A7" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>9</v>
@@ -1439,21 +1439,21 @@
         <v>10</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="31">
       <c r="A8" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>9</v>
@@ -1462,21 +1462,21 @@
         <v>10</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="31">
       <c r="A9" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
@@ -1485,13 +1485,13 @@
         <v>10</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1513,21 +1513,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562F5F3D-E2EA-9240-9A70-317BC054BC3A}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="47" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="E1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="29.4609375" customWidth="1"/>
-    <col min="3" max="3" width="9.15234375" customWidth="1"/>
-    <col min="4" max="4" width="46.3046875" customWidth="1"/>
-    <col min="5" max="5" width="60.84375" customWidth="1"/>
-    <col min="6" max="6" width="49.15234375" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="51.08203125" customWidth="1"/>
+    <col min="5" max="5" width="60.83203125" customWidth="1"/>
+    <col min="6" max="6" width="49.1640625" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
-    <col min="8" max="8" width="34.3046875" customWidth="1"/>
-    <col min="9" max="9" width="21.69140625" customWidth="1"/>
+    <col min="8" max="8" width="34.33203125" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1">
@@ -1547,7 +1547,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1559,10 +1559,10 @@
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="31">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="32">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1576,16 +1576,16 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1593,19 +1593,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1613,19 +1613,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="66" customHeight="1">
@@ -1633,19 +1633,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="61" customHeight="1">
@@ -1653,71 +1653,71 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="43.5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="124">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="128">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" t="s">
         <v>33</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>34</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="29">
@@ -1725,19 +1725,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I9" s="3"/>
     </row>
@@ -1746,42 +1746,42 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="120">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="135">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>